<commit_message>
updated database proposal & colored requirements
</commit_message>
<xml_diff>
--- a/doc/requirements/HerediVar_requirement_colored.xlsx
+++ b/doc/requirements/HerediVar_requirement_colored.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nacl2svm1.ukt.ad.local\ahdoebm1\UserProfile\Desktop\Workspace\HerediVar\doc\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E5655-B58C-4A74-987D-E6A5299E5340}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59AFCD9-C83C-4D12-8FCC-A06AAA334CA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="90" windowWidth="26445" windowHeight="12885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>AF, pop_max, #hom/#hemi</t>
   </si>
   <si>
     <t>genomAD</t>
@@ -413,6 +410,9 @@
   </si>
   <si>
     <t>http://bioinfo.univ-rouen.fr/HExoSplice_submit/index.php</t>
+  </si>
+  <si>
+    <t>AF, pop_max, #hom/#hemi/#het/#wt, AC</t>
   </si>
 </sst>
 </file>
@@ -894,7 +894,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,10 +905,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -956,7 +956,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -980,20 +980,20 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1038,7 @@
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>74</v>
@@ -1049,7 +1049,7 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -1067,7 +1067,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B5" t="s">
@@ -1086,7 +1086,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C7" t="s">
@@ -1094,11 +1094,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
@@ -1106,10 +1106,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>64</v>
@@ -1160,13 +1160,13 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1237,20 +1237,20 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,25 +1259,25 @@
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
         <v>74</v>
@@ -1334,10 +1334,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
         <v>119</v>
-      </c>
-      <c r="B32" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1382,39 +1382,39 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
         <v>107</v>
-      </c>
-      <c r="C41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
         <v>112</v>
-      </c>
-      <c r="B43" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>1</v>
@@ -1426,7 +1426,7 @@
         <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1442,18 +1442,18 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1469,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1490,7 +1490,7 @@
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>1</v>
@@ -1518,7 +1518,7 @@
         <v>20</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C60" s="4"/>
     </row>

</xml_diff>

<commit_message>
update api endpoints (#23) & requirements sheet
</commit_message>
<xml_diff>
--- a/doc/requirements/HerediVar_requirement_colored.xlsx
+++ b/doc/requirements/HerediVar_requirement_colored.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marc\GIT\+GC-HBOC\HerediVar\doc\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nacl2svm1.ukt.ad.local\ahdoebm1\UserProfile\Desktop\doc\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20F1329-E5EB-4CFC-B518-ECB01949CA43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05B8C2F-0607-4801-A696-BF49A8B88949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="90" windowWidth="26445" windowHeight="12885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="137">
   <si>
     <t>ClinVar</t>
   </si>
@@ -99,18 +99,9 @@
     <t>Variantenliste</t>
   </si>
   <si>
-    <t xml:space="preserve">Bereits in Leipzig vorhandene Bemerkungen der TF </t>
-  </si>
-  <si>
-    <t>https://p53.iarc.fr/TP53GeneVariations.aspx</t>
-  </si>
-  <si>
     <t>ein LikelyhoodRatio für alle Daten die verfügbar sind</t>
   </si>
   <si>
-    <t>Bewertung und Kommentar</t>
-  </si>
-  <si>
     <t>Export-Möglichkeiten einzelner Daten, um diese in den jeweiligen zentrumseigenen Datensammlungen abspeichern zu können. VCF-Export per Email/HTTPs</t>
   </si>
   <si>
@@ -126,12 +117,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Seq-ID aus HerediCare</t>
-  </si>
-  <si>
-    <t>HerediCare</t>
-  </si>
-  <si>
     <t>für Ensebl, RefSeq,LRG, MANE Transkripte; Highlighen von preferred transcripts (MANE select, etc).</t>
   </si>
   <si>
@@ -192,36 +177,21 @@
     <t>clinical Significance</t>
   </si>
   <si>
-    <t>IARC TP53</t>
-  </si>
-  <si>
-    <t>(functional) prediction + clinical classification</t>
-  </si>
-  <si>
     <t>Cancer hotspots</t>
   </si>
   <si>
-    <t>hotspots</t>
-  </si>
-  <si>
     <t>LYNCH genes: MAPP / PP2</t>
   </si>
   <si>
     <t>https://gnomad.broadinstitute.org/downloads</t>
   </si>
   <si>
-    <t>http://cancerhospots.org</t>
-  </si>
-  <si>
     <t>Literatur: PubMed-Ids</t>
   </si>
   <si>
     <t>Google-Suche (Variatensuche mit 1-Buchstaben, 3-Buchstaben, rs-Nummer)</t>
   </si>
   <si>
-    <t>VEP, ClinVar?, Mastermind?</t>
-  </si>
-  <si>
     <t>Algorithmus Hannover</t>
   </si>
   <si>
@@ -231,12 +201,6 @@
     <t>Score + PDF</t>
   </si>
   <si>
-    <t>Allele frequency / depth</t>
-  </si>
-  <si>
-    <t>Sobald in HerediCare abgebildet</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -285,9 +249,6 @@
     <t>Export der für die Bewertung der jeweiligen Variante relevanten Informationen als Zusammenfassung (PDF)</t>
   </si>
   <si>
-    <t>Strukturiere Erfassung der Hauptkriterien die zur TF-Klassifikation führten</t>
-  </si>
-  <si>
     <t>Automatisierte Klassifizierung von Varianten (Hannover) &gt; Erkennung von Konflikten mit bisheriger Klassifizierung + Priosisierung wahrscheinlicher Klasse 4/5 Varianten</t>
   </si>
   <si>
@@ -309,9 +270,6 @@
     <t>http://priors.hci.utah.edu/PRIORS/BRCA/indexBRCA2.php</t>
   </si>
   <si>
-    <t>tool?</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://tp53.isb-cgc.org/ </t>
   </si>
   <si>
@@ -345,9 +303,6 @@
     <t>Gen</t>
   </si>
   <si>
-    <t>alle VUS, regelmäßig importieren (prüfen ob Valide vor Import!!!)</t>
-  </si>
-  <si>
     <t>In wievielen Familien gefunden? In wievielen Fällen gefunden?</t>
   </si>
   <si>
@@ -360,11 +315,35 @@
     <t>Anzahl Träger BC, OC, BCOC, nicht erkrankte + age at onset/diagnosis of disease + Ethnie + Geschlecht (Personenspezifische Daten höchstens temporär, speziell für TP53 [age at onset+Tumortyp+Familie])</t>
   </si>
   <si>
-    <t>Varianten-Zahl in Zentren</t>
+    <t>TP53 noch prüfen ob relevant &gt; Gunnar</t>
+  </si>
+  <si>
+    <t>http://bioinfo.univ-rouen.fr/HExoSplice_submit/index.php</t>
+  </si>
+  <si>
+    <t>AF, pop_max, #hom/#hemi/#het/#wt, AC</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Topmed</t>
+  </si>
+  <si>
+    <t>https://bravo.sph.umich.edu/freeze8/hg38/</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Fragen</t>
+  </si>
+  <si>
+    <t>VariationID</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">#Fälle pro Zentrum, optional: #Tumor-Fälle + #Nicht-Tumor-Fälle für bestimmte Gene (Core-Gene, MLH1, MSH2, MSH6, STK11, PTEN, </t>
+      <t xml:space="preserve">erst nur kleine Varianten, </t>
     </r>
     <r>
       <rPr>
@@ -374,7 +353,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>...</t>
+      <t>CNVs und SVs später</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PFAM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (PFAM protein domains für RefSeq consequences?)</t>
     </r>
     <r>
       <rPr>
@@ -384,73 +378,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>TP53 noch prüfen ob relevant &gt; Gunnar</t>
-  </si>
-  <si>
-    <t>http://bioinfo.univ-rouen.fr/HExoSplice_submit/index.php</t>
-  </si>
-  <si>
-    <t>AF, pop_max, #hom/#hemi/#het/#wt, AC</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Topmed</t>
-  </si>
-  <si>
-    <t>ENIGMA</t>
-  </si>
-  <si>
-    <t>https://bravo.sph.umich.edu/freeze8/hg38/</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>same as IARC TP53! -&gt; they moved the database</t>
-  </si>
-  <si>
-    <t>Identifiziert die Seqid den Fall/Patient?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Rückspielen von Daten nach HerediCare sonst nicht möglich; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vorsicht es könnten mehrere Seq-IDs für die selbe Variaten da sein</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =&gt; Prüfen!</t>
-    </r>
-  </si>
-  <si>
-    <t>Fragen</t>
-  </si>
-  <si>
-    <t>VariationID</t>
-  </si>
-  <si>
-    <r>
-      <t>PFAM,</t>
+      <t>,</t>
     </r>
     <r>
       <rPr>
@@ -494,8 +422,32 @@
     </r>
   </si>
   <si>
+    <t>http://cancerhotspots.org</t>
+  </si>
+  <si>
+    <t>hotspots (AF, AC, tumor-type)</t>
+  </si>
+  <si>
+    <t>priors.hci.utah.edu/PRIORS/BRCA/viewer.php?gene=BRCA2&amp;subs_type=HGVS&amp;nt_pos=796</t>
+  </si>
+  <si>
+    <t>BRCA1/2: HCI Cancer Sesceptibility Genes Prior Probabilities of Pathogenicity?</t>
+  </si>
+  <si>
+    <t>autor, titel, journal, pmid</t>
+  </si>
+  <si>
+    <t>Uniprot?, Handkuriert?</t>
+  </si>
+  <si>
+    <t>Über Webinterface?</t>
+  </si>
+  <si>
+    <t>Bisher nur VEP</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">erst nur kleine Varianten, </t>
+      <t>VEP,</t>
     </r>
     <r>
       <rPr>
@@ -505,20 +457,68 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CNVs und SVs später</t>
+      <t xml:space="preserve"> ClinVar?</t>
     </r>
   </si>
   <si>
-    <t>Variante, Genombuild</t>
+    <t>https://topmed.nhlbi.nih.gov/topmed-data-access-scientific-community --&gt; download schwierig!</t>
+  </si>
+  <si>
+    <t>priors</t>
+  </si>
+  <si>
+    <t>insight</t>
+  </si>
+  <si>
+    <t>http://www.insight-database.org/classifications/</t>
+  </si>
+  <si>
+    <t>Combined phenotype score</t>
+  </si>
+  <si>
+    <t>enigma</t>
+  </si>
+  <si>
+    <t>Varianten ohne SeqID in HerediCare einfügen</t>
+  </si>
+  <si>
+    <t>Special User priviliges</t>
+  </si>
+  <si>
+    <t>PHANTM</t>
+  </si>
+  <si>
+    <t>Strukturiere Erfassung der Hauptkriterien die zur TF-Klassifikation führten (PDF stand der Annotationen + modellierung der ACMG Kriterien)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Variantensuche nach HGVSc &amp; p und nach gen und nach chromosomal range und ….</t>
+  </si>
+  <si>
+    <t>MLH1 MSH2 MSH6 prior (evtl. noch pms2 aus einer anderen datenbank: vllt. insight.org?)</t>
+  </si>
+  <si>
+    <t>http://priors.hci.utah.edu/PRIORS/BRCA/indexMLH1.php</t>
+  </si>
+  <si>
+    <t>same as IARC TP53! -&gt; they moved the database ((functional) prediction + clinical classification)</t>
+  </si>
+  <si>
+    <t>alle VUS, regelmäßig importieren (prüfen ob Valide vor Import!!!)</t>
+  </si>
+  <si>
+    <t>Klassifizierung in HerediCare</t>
+  </si>
+  <si>
+    <t>Klassifikationen der Zentren und der VUS-Taskforce? Erstmeldendes Zentrum hervorheben</t>
   </si>
   <si>
     <t>Zentrum, Klasse, Kommentar</t>
   </si>
   <si>
-    <t>Klassifizierung in HerediCare</t>
-  </si>
-  <si>
-    <t>Klassifikationen der Zentren und der VUS-Taskforce? Erstmeldendes Zentrum hervorheben</t>
+    <t>Variante (VCF), Genombuild, SeqID (wenns das nicht gibt nicht importieren) + Allele frequency / depth / genotype</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -673,6 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Gut" xfId="5" builtinId="26"/>
@@ -1021,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,10 +1036,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1046,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,7 +1063,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1070,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1079,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1086,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1102,7 +1103,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1110,20 +1111,28 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1133,18 +1142,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:D56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="75.85546875" customWidth="1"/>
+    <col min="2" max="2" width="69" customWidth="1"/>
     <col min="3" max="3" width="170.85546875" customWidth="1"/>
-    <col min="4" max="4" width="59.7109375" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
     <col min="5" max="5" width="48.85546875" customWidth="1"/>
     <col min="6" max="6" width="54.5703125" customWidth="1"/>
     <col min="7" max="7" width="40.28515625" bestFit="1" customWidth="1"/>
@@ -1154,486 +1163,500 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="B3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
-        <v>124</v>
+      <c r="C3" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>70</v>
+      <c r="A4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="6" t="s">
-        <v>41</v>
+      <c r="A8" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
+      <c r="A13" s="11"/>
+      <c r="B13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>115</v>
+      <c r="A15" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>117</v>
-      </c>
+      <c r="A16" s="14"/>
       <c r="B16" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>117</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
       <c r="B17" s="9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="B18" s="9" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="9" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="9" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
-      <c r="B21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
+      <c r="B21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="4" t="s">
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="2" t="s">
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>1</v>
@@ -1645,10 +1668,10 @@
         <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
@@ -1657,7 +1680,7 @@
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
@@ -1665,7 +1688,7 @@
         <v>4</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D52" s="9"/>
     </row>
@@ -1674,46 +1697,37 @@
         <v>3</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>114</v>
+      <c r="B55" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="5" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>1</v>
@@ -1727,6 +1741,9 @@
       <c r="C59" t="s">
         <v>16</v>
       </c>
+      <c r="D59" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
@@ -1741,39 +1758,40 @@
         <v>19</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>114</v>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D19" r:id="rId1" xr:uid="{514F072A-0C80-4FE8-9EAF-8A60541AC6A7}"/>
-    <hyperlink ref="D20" r:id="rId2" xr:uid="{ADCAE1A5-854F-4727-BC29-6F94079E7729}"/>
-    <hyperlink ref="D21" r:id="rId3" xr:uid="{7668369E-A38D-4F13-B3B8-88387800ACF2}"/>
-    <hyperlink ref="D22" r:id="rId4" xr:uid="{F1F9E258-CBE3-46A5-9B46-396633557A34}"/>
-    <hyperlink ref="D25" r:id="rId5" xr:uid="{22ED4FAD-78D0-4C9A-816A-3EAE0A02381D}"/>
-    <hyperlink ref="D15" r:id="rId6" xr:uid="{681B41E2-3972-4752-8139-0F35C10A111A}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{4194C509-4ADF-4B22-B4CE-D05B04FED622}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{D88967BC-5914-4362-8D4E-50F275A7AE79}"/>
-    <hyperlink ref="D16" r:id="rId9" xr:uid="{6F5237BC-3FF8-4E79-8A17-14ED4DFD3BF1}"/>
-    <hyperlink ref="D17" r:id="rId10" xr:uid="{328A7DC6-5F4E-4A49-AC20-D3E6CAF47529}"/>
-    <hyperlink ref="D18" r:id="rId11" xr:uid="{259E0015-A445-4E5E-9837-015E0E9E9A74}"/>
-    <hyperlink ref="D26" r:id="rId12" xr:uid="{2071B899-D471-4707-A1F0-E4A03608E151}"/>
-    <hyperlink ref="D33" r:id="rId13" xr:uid="{9942CE00-FD90-4A7B-BFF8-A140CC674E55}"/>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{514F072A-0C80-4FE8-9EAF-8A60541AC6A7}"/>
+    <hyperlink ref="D18" r:id="rId2" xr:uid="{7668369E-A38D-4F13-B3B8-88387800ACF2}"/>
+    <hyperlink ref="D19" r:id="rId3" xr:uid="{F1F9E258-CBE3-46A5-9B46-396633557A34}"/>
+    <hyperlink ref="D22" r:id="rId4" xr:uid="{22ED4FAD-78D0-4C9A-816A-3EAE0A02381D}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{681B41E2-3972-4752-8139-0F35C10A111A}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{4194C509-4ADF-4B22-B4CE-D05B04FED622}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{D88967BC-5914-4362-8D4E-50F275A7AE79}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{6F5237BC-3FF8-4E79-8A17-14ED4DFD3BF1}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{328A7DC6-5F4E-4A49-AC20-D3E6CAF47529}"/>
+    <hyperlink ref="D16" r:id="rId10" xr:uid="{259E0015-A445-4E5E-9837-015E0E9E9A74}"/>
+    <hyperlink ref="D23" r:id="rId11" xr:uid="{2071B899-D471-4707-A1F0-E4A03608E151}"/>
+    <hyperlink ref="D29" r:id="rId12" xr:uid="{9942CE00-FD90-4A7B-BFF8-A140CC674E55}"/>
+    <hyperlink ref="D44" r:id="rId13" display="http://priors.hci.utah.edu/PRIORS/BRCA/viewer.php?gene=BRCA2&amp;subs_type=HGVS&amp;nt_pos=796" xr:uid="{AC34915D-AE1E-487D-81E8-E5973505C316}"/>
+    <hyperlink ref="C19" r:id="rId14" display="http://agvgd.hci.utah.edu/disclaimer.php -&gt; dieser algorithmus wurde von denen ausgeführt für alle substitutionen aus BRCA1&amp;2" xr:uid="{EAA984C8-46C7-4EFC-A495-369AD8439213}"/>
+    <hyperlink ref="C29" r:id="rId15" xr:uid="{F20FA793-39FA-40E2-9435-D0318EA98095}"/>
+    <hyperlink ref="D47" r:id="rId16" xr:uid="{DDA0CD0E-7875-450D-B39A-EBDB15F68253}"/>
+    <hyperlink ref="D20" r:id="rId17" xr:uid="{E6E19F7D-F656-4BAC-9763-AE9AE307E96C}"/>
+    <hyperlink ref="D21" r:id="rId18" xr:uid="{2BA7A493-953A-4AEB-9554-81D2FA3C914F}"/>
+    <hyperlink ref="D40" r:id="rId19" xr:uid="{5118547B-3B27-4F45-8797-7A9907C4116F}"/>
+    <hyperlink ref="D41" r:id="rId20" xr:uid="{66963962-A9DE-4DAA-AF6D-9BA47B8CB5E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>